<commit_message>
feat: generate cross-validation results and comparison metrics for multiple model runs
</commit_message>
<xml_diff>
--- a/results/cv_results/multi_condition_best_per_run_summary.xlsx
+++ b/results/cv_results/multi_condition_best_per_run_summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>run_dir</t>
   </si>
@@ -67,6 +67,21 @@
     <t>run_g3</t>
   </si>
   <si>
+    <t>run_g4</t>
+  </si>
+  <si>
+    <t>run_g5</t>
+  </si>
+  <si>
+    <t>run_g2</t>
+  </si>
+  <si>
+    <t>run_g1</t>
+  </si>
+  <si>
+    <t>run_g6</t>
+  </si>
+  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -79,7 +94,37 @@
     <t>anom_swh_min_swan &gt; t1 AND swh_max_swan &gt; t2</t>
   </si>
   <si>
+    <t>swh_p80_swan &gt; t1 AND anom_swh_mean_deseasonalized_detrended &gt; t2</t>
+  </si>
+  <si>
+    <t>swh_p80_swan &gt; t1 AND swh_max_swan &gt; t2</t>
+  </si>
+  <si>
+    <t>anom_swh_min_waverys &gt; t1 AND anom_swh_max_waverys &gt; t2</t>
+  </si>
+  <si>
+    <t>anom_swe_min &gt; t1 AND anom_swh_max_waverys &gt; t2</t>
+  </si>
+  <si>
+    <t>anom_swh_min_waverys &gt; t1 AND anom_swh_p80_swan &gt; t2</t>
+  </si>
+  <si>
     <t>enhanced_multi_rule_summary_20250711_143735.csv</t>
+  </si>
+  <si>
+    <t>enhanced_multi_rule_summary_20250714_121146.csv</t>
+  </si>
+  <si>
+    <t>enhanced_multi_rule_summary_20250714_124208.csv</t>
+  </si>
+  <si>
+    <t>enhanced_multi_rule_summary_20250713_172447.csv</t>
+  </si>
+  <si>
+    <t>enhanced_multi_rule_summary_20250713_170835.csv</t>
+  </si>
+  <si>
+    <t>enhanced_multi_rule_summary_20250714_130045.csv</t>
   </si>
 </sst>
 </file>
@@ -437,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,13 +543,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E2">
         <v>0.3307086614173228</v>
@@ -519,28 +564,28 @@
         <v>21</v>
       </c>
       <c r="I2">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J2">
-        <v>2451</v>
+        <v>2245</v>
       </c>
       <c r="K2">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="L2">
-        <v>0.3043478260869565</v>
+        <v>0.3134328358208955</v>
       </c>
       <c r="M2">
-        <v>0.3620689655172414</v>
+        <v>0.42</v>
       </c>
       <c r="N2">
-        <v>0.9667579194368401</v>
+        <v>0.9679624092268262</v>
       </c>
       <c r="O2">
-        <v>0.3307086614173229</v>
+        <v>0.358974358974359</v>
       </c>
       <c r="P2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -548,49 +593,299 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E3">
-        <v>0.3307086614173228</v>
+        <v>0.5521064301552105</v>
       </c>
       <c r="F3">
-        <v>1711241.429632653</v>
+        <v>5601398</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
+        <v>249</v>
+      </c>
+      <c r="I3">
+        <v>269</v>
+      </c>
+      <c r="J3">
+        <v>1904</v>
+      </c>
+      <c r="K3">
+        <v>135</v>
+      </c>
+      <c r="L3">
+        <v>0.4806949806949807</v>
+      </c>
+      <c r="M3">
+        <v>0.6484375</v>
+      </c>
+      <c r="N3">
+        <v>0.8420023464998044</v>
+      </c>
+      <c r="O3">
+        <v>0.5521064301552107</v>
+      </c>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4">
+        <v>0.4281524926686216</v>
+      </c>
+      <c r="F4">
+        <v>570803.0660659341</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>73</v>
+      </c>
+      <c r="I4">
+        <v>55</v>
+      </c>
+      <c r="J4">
+        <v>2289</v>
+      </c>
+      <c r="K4">
+        <v>140</v>
+      </c>
+      <c r="L4">
+        <v>0.5703125</v>
+      </c>
+      <c r="M4">
+        <v>0.3427230046948357</v>
+      </c>
+      <c r="N4">
+        <v>0.9237387563551036</v>
+      </c>
+      <c r="O4">
+        <v>0.4281524926686217</v>
+      </c>
+      <c r="P4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5">
+        <v>0.296875</v>
+      </c>
+      <c r="F5">
+        <v>243425.9018571429</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>19</v>
+      </c>
+      <c r="I5">
+        <v>56</v>
+      </c>
+      <c r="J5">
+        <v>2448</v>
+      </c>
+      <c r="K5">
+        <v>34</v>
+      </c>
+      <c r="L5">
+        <v>0.2533333333333334</v>
+      </c>
+      <c r="M5">
+        <v>0.3584905660377358</v>
+      </c>
+      <c r="N5">
+        <v>0.9648025029331248</v>
+      </c>
+      <c r="O5">
+        <v>0.296875</v>
+      </c>
+      <c r="P5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>0.4583333333333333</v>
+      </c>
+      <c r="F6">
+        <v>81190.8</v>
+      </c>
+      <c r="G6">
+        <v>0.015</v>
+      </c>
+      <c r="H6">
+        <v>22</v>
+      </c>
+      <c r="I6">
+        <v>27</v>
+      </c>
+      <c r="J6">
+        <v>2483</v>
+      </c>
+      <c r="K6">
+        <v>25</v>
+      </c>
+      <c r="L6">
+        <v>0.4489795918367347</v>
+      </c>
+      <c r="M6">
+        <v>0.4680851063829787</v>
+      </c>
+      <c r="N6">
+        <v>0.979663668361361</v>
+      </c>
+      <c r="O6">
+        <v>0.4583333333333333</v>
+      </c>
+      <c r="P6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="I3">
-        <v>48</v>
-      </c>
-      <c r="J3">
-        <v>2451</v>
-      </c>
-      <c r="K3">
-        <v>37</v>
-      </c>
-      <c r="L3">
-        <v>0.3043478260869565</v>
-      </c>
-      <c r="M3">
-        <v>0.3620689655172414</v>
-      </c>
-      <c r="N3">
-        <v>0.9667579194368401</v>
-      </c>
-      <c r="O3">
-        <v>0.3307086614173229</v>
-      </c>
-      <c r="P3" t="s">
-        <v>17</v>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>0.2681451612903225</v>
+      </c>
+      <c r="F7">
+        <v>3237740.665735714</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>133</v>
+      </c>
+      <c r="I7">
+        <v>589</v>
+      </c>
+      <c r="J7">
+        <v>1705</v>
+      </c>
+      <c r="K7">
+        <v>137</v>
+      </c>
+      <c r="L7">
+        <v>0.1842105263157895</v>
+      </c>
+      <c r="M7">
+        <v>0.4925925925925926</v>
+      </c>
+      <c r="N7">
+        <v>0.7168486739469578</v>
+      </c>
+      <c r="O7">
+        <v>0.2681451612903226</v>
+      </c>
+      <c r="P7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>2.334321078864811</v>
+      </c>
+      <c r="F8">
+        <v>11445799.86329144</v>
+      </c>
+      <c r="G8">
+        <v>0.015</v>
+      </c>
+      <c r="H8">
+        <v>517</v>
+      </c>
+      <c r="I8">
+        <v>1042</v>
+      </c>
+      <c r="J8">
+        <v>13074</v>
+      </c>
+      <c r="K8">
+        <v>500</v>
+      </c>
+      <c r="L8">
+        <v>2.250963768001734</v>
+      </c>
+      <c r="M8">
+        <v>2.730328769708143</v>
+      </c>
+      <c r="N8">
+        <v>5.395018357323178</v>
+      </c>
+      <c r="O8">
+        <v>2.362586776421847</v>
+      </c>
+      <c r="P8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated AEP metric extraction
</commit_message>
<xml_diff>
--- a/results/cv_results/multi_condition_best_per_run_summary.xlsx
+++ b/results/cv_results/multi_condition_best_per_run_summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>run_dir</t>
   </si>
@@ -37,6 +37,12 @@
     <t>zero_prob</t>
   </si>
   <si>
+    <t>thresholds</t>
+  </si>
+  <si>
+    <t>source_file</t>
+  </si>
+  <si>
     <t>obs_tp</t>
   </si>
   <si>
@@ -61,9 +67,6 @@
     <t>obs_f1</t>
   </si>
   <si>
-    <t>source_file</t>
-  </si>
-  <si>
     <t>run_g3</t>
   </si>
   <si>
@@ -76,12 +79,24 @@
     <t>run_g2</t>
   </si>
   <si>
+    <t>run_g9</t>
+  </si>
+  <si>
+    <t>run_g7</t>
+  </si>
+  <si>
     <t>run_g1</t>
   </si>
   <si>
     <t>run_g6</t>
   </si>
   <si>
+    <t>run_g8</t>
+  </si>
+  <si>
+    <t>run_g10</t>
+  </si>
+  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -91,7 +106,7 @@
     <t>double_AND</t>
   </si>
   <si>
-    <t>anom_swh_min_swan &gt; t1 AND swh_max_swan &gt; t2</t>
+    <t>swh_max_swan &gt; t1 AND anom_swh_median_persistence_2 &gt; t2</t>
   </si>
   <si>
     <t>swh_p80_swan &gt; t1 AND anom_swh_mean_deseasonalized_detrended &gt; t2</t>
@@ -103,28 +118,82 @@
     <t>anom_swh_min_waverys &gt; t1 AND anom_swh_max_waverys &gt; t2</t>
   </si>
   <si>
-    <t>anom_swe_min &gt; t1 AND anom_swh_max_waverys &gt; t2</t>
+    <t>swh_max_swan &gt; t1 AND anom_swh_p80_swan &gt; t2</t>
+  </si>
+  <si>
+    <t>anom_swe_mean &gt; t1 AND swh_max_swan &gt; t2</t>
+  </si>
+  <si>
+    <t>anom_swe_min &gt; t1 AND anom_swe_max &gt; t2</t>
   </si>
   <si>
     <t>anom_swh_min_waverys &gt; t1 AND anom_swh_p80_swan &gt; t2</t>
   </si>
   <si>
-    <t>enhanced_multi_rule_summary_20250711_143735.csv</t>
-  </si>
-  <si>
-    <t>enhanced_multi_rule_summary_20250714_121146.csv</t>
-  </si>
-  <si>
-    <t>enhanced_multi_rule_summary_20250714_124208.csv</t>
-  </si>
-  <si>
-    <t>enhanced_multi_rule_summary_20250713_172447.csv</t>
-  </si>
-  <si>
-    <t>enhanced_multi_rule_summary_20250713_170835.csv</t>
+    <t>swh_max_swan &gt; t1 AND swh_p80_swan &gt; t2</t>
+  </si>
+  <si>
+    <t>swh_max_swan &gt; t1 AND anom_swh_max_swan &gt; t2</t>
+  </si>
+  <si>
+    <t>(np.float64(1.58), np.float64(0.2918489530208332))</t>
+  </si>
+  <si>
+    <t>(np.float64(1.7274392652511599), np.float64(0.07092036516966926))</t>
+  </si>
+  <si>
+    <t>(np.float64(2.426971555999999), np.float64(1.2128571))</t>
+  </si>
+  <si>
+    <t>(np.float64(0.20771093750000003), np.float64(0.4388984374999997))</t>
+  </si>
+  <si>
+    <t>(np.float64(1.9166666), np.float64(0.1850487195833333))</t>
+  </si>
+  <si>
+    <t>(np.float64(0.01015625), np.float64(1.34))</t>
+  </si>
+  <si>
+    <t>(np.float64(0.13375), np.float64(0.299828125))</t>
+  </si>
+  <si>
+    <t>(np.float64(-0.04634960937499997), np.float64(0.14617807558333323))</t>
+  </si>
+  <si>
+    <t>(np.float64(2.0149999), np.float64(1.94670002))</t>
+  </si>
+  <si>
+    <t>(np.float64(1.953333395), np.float64(0.26049826140624993))</t>
+  </si>
+  <si>
+    <t>enhanced_multi_rule_complete_summary_20250718_162648.csv</t>
+  </si>
+  <si>
+    <t>enhanced_multi_rule_complete_summary_20250718_164905.csv</t>
+  </si>
+  <si>
+    <t>enhanced_multi_rule_complete_summary_20250718_164927.csv</t>
+  </si>
+  <si>
+    <t>enhanced_multi_rule_complete_summary_20250718_162601.csv</t>
+  </si>
+  <si>
+    <t>enhanced_multi_rule_summary_20250717_144034.csv</t>
+  </si>
+  <si>
+    <t>enhanced_multi_rule_summary_20250717_140021.csv</t>
+  </si>
+  <si>
+    <t>enhanced_multi_rule_complete_summary_20250718_143556.csv</t>
   </si>
   <si>
     <t>enhanced_multi_rule_summary_20250714_130045.csv</t>
+  </si>
+  <si>
+    <t>enhanced_multi_rule_summary_20250717_142644.csv</t>
+  </si>
+  <si>
+    <t>enhanced_multi_rule_complete_summary_20250718_130359.csv</t>
   </si>
 </sst>
 </file>
@@ -482,13 +551,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,119 +606,128 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E2">
-        <v>0.3307086614173228</v>
+        <v>0.3508771929824561</v>
       </c>
       <c r="F2">
-        <v>1711241.429632653</v>
+        <v>1693035.868946939</v>
       </c>
       <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>21</v>
-      </c>
-      <c r="I2">
-        <v>46</v>
+        <v>0.001</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>50</v>
       </c>
       <c r="J2">
-        <v>2245</v>
+        <v>20</v>
       </c>
       <c r="K2">
+        <v>44</v>
+      </c>
+      <c r="L2">
+        <v>2247</v>
+      </c>
+      <c r="M2">
+        <v>30</v>
+      </c>
+      <c r="N2">
+        <v>0.3125</v>
+      </c>
+      <c r="O2">
+        <v>0.4</v>
+      </c>
+      <c r="P2">
+        <v>0.9683895771038018</v>
+      </c>
+      <c r="Q2">
+        <v>0.3508771929824561</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="L2">
-        <v>0.3134328358208955</v>
-      </c>
-      <c r="M2">
-        <v>0.42</v>
-      </c>
-      <c r="N2">
-        <v>0.9679624092268262</v>
-      </c>
-      <c r="O2">
-        <v>0.358974358974359</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="D3" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
       </c>
       <c r="E3">
         <v>0.5521064301552105</v>
       </c>
       <c r="F3">
-        <v>5601398</v>
+        <v>5550496.6</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3">
         <v>249</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>269</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>1904</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>135</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>0.4806949806949807</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>0.6484375</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>0.8420023464998044</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>0.5521064301552107</v>
       </c>
-      <c r="P3" t="s">
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
       </c>
       <c r="E4">
         <v>0.4281524926686216</v>
@@ -660,232 +738,459 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4">
         <v>73</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>55</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>2289</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>140</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>0.5703125</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>0.3427230046948357</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>0.9237387563551036</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>0.4281524926686217</v>
       </c>
-      <c r="P4" t="s">
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
       </c>
       <c r="E5">
         <v>0.296875</v>
       </c>
       <c r="F5">
-        <v>243425.9018571429</v>
+        <v>242271.1520485715</v>
       </c>
       <c r="G5">
+        <v>0.001</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5">
+        <v>19</v>
+      </c>
+      <c r="K5">
+        <v>56</v>
+      </c>
+      <c r="L5">
+        <v>2448</v>
+      </c>
+      <c r="M5">
+        <v>34</v>
+      </c>
+      <c r="N5">
+        <v>0.2533333333333334</v>
+      </c>
+      <c r="O5">
+        <v>0.3584905660377358</v>
+      </c>
+      <c r="P5">
+        <v>0.9648025029331248</v>
+      </c>
+      <c r="Q5">
+        <v>0.296875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6">
+        <v>0.640194489465154</v>
+      </c>
+      <c r="F6">
+        <v>118713.7737142857</v>
+      </c>
+      <c r="G6">
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>19</v>
-      </c>
-      <c r="I5">
-        <v>56</v>
-      </c>
-      <c r="J5">
-        <v>2448</v>
-      </c>
-      <c r="K5">
-        <v>34</v>
-      </c>
-      <c r="L5">
-        <v>0.2533333333333334</v>
-      </c>
-      <c r="M5">
-        <v>0.3584905660377358</v>
-      </c>
-      <c r="N5">
-        <v>0.9648025029331248</v>
-      </c>
-      <c r="O5">
-        <v>0.296875</v>
-      </c>
-      <c r="P5" t="s">
-        <v>34</v>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6">
+        <v>395</v>
+      </c>
+      <c r="K6">
+        <v>332</v>
+      </c>
+      <c r="L6">
+        <v>1722</v>
+      </c>
+      <c r="M6">
+        <v>112</v>
+      </c>
+      <c r="N6">
+        <v>0.5433287482806052</v>
+      </c>
+      <c r="O6">
+        <v>0.7790927021696252</v>
+      </c>
+      <c r="P6">
+        <v>0.8266302225693088</v>
+      </c>
+      <c r="Q6">
+        <v>0.640194489465154</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
         <v>29</v>
       </c>
-      <c r="E6">
-        <v>0.4583333333333333</v>
-      </c>
-      <c r="F6">
-        <v>81190.8</v>
-      </c>
-      <c r="G6">
-        <v>0.015</v>
-      </c>
-      <c r="H6">
-        <v>22</v>
-      </c>
-      <c r="I6">
-        <v>27</v>
-      </c>
-      <c r="J6">
-        <v>2483</v>
-      </c>
-      <c r="K6">
-        <v>25</v>
-      </c>
-      <c r="L6">
-        <v>0.4489795918367347</v>
-      </c>
-      <c r="M6">
-        <v>0.4680851063829787</v>
-      </c>
-      <c r="N6">
-        <v>0.979663668361361</v>
-      </c>
-      <c r="O6">
-        <v>0.4583333333333333</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="D7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
       <c r="E7">
-        <v>0.2681451612903225</v>
+        <v>0.4670781893004115</v>
       </c>
       <c r="F7">
-        <v>3237740.665735714</v>
+        <v>237144.8314285714</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7">
+      <c r="H7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7">
+        <v>227</v>
+      </c>
+      <c r="K7">
+        <v>396</v>
+      </c>
+      <c r="L7">
+        <v>1812</v>
+      </c>
+      <c r="M7">
+        <v>122</v>
+      </c>
+      <c r="N7">
+        <v>0.3643659711075442</v>
+      </c>
+      <c r="O7">
+        <v>0.6504297994269341</v>
+      </c>
+      <c r="P7">
+        <v>0.7974188502150958</v>
+      </c>
+      <c r="Q7">
+        <v>0.4670781893004115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8">
+        <v>0.4504504504504504</v>
+      </c>
+      <c r="F8">
+        <v>103494.53</v>
+      </c>
+      <c r="G8">
+        <v>0.008750000000000001</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8">
+        <v>25</v>
+      </c>
+      <c r="K8">
+        <v>39</v>
+      </c>
+      <c r="L8">
+        <v>2471</v>
+      </c>
+      <c r="M8">
+        <v>22</v>
+      </c>
+      <c r="N8">
+        <v>0.390625</v>
+      </c>
+      <c r="O8">
+        <v>0.5319148936170213</v>
+      </c>
+      <c r="P8">
+        <v>0.9761439186546734</v>
+      </c>
+      <c r="Q8">
+        <v>0.4504504504504505</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9">
+        <v>0.2681451612903225</v>
+      </c>
+      <c r="F9">
+        <v>3237740.665735714</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9">
         <v>133</v>
       </c>
-      <c r="I7">
+      <c r="K9">
         <v>589</v>
       </c>
-      <c r="J7">
+      <c r="L9">
         <v>1705</v>
       </c>
-      <c r="K7">
+      <c r="M9">
         <v>137</v>
       </c>
-      <c r="L7">
+      <c r="N9">
         <v>0.1842105263157895</v>
       </c>
-      <c r="M7">
+      <c r="O9">
         <v>0.4925925925925926</v>
       </c>
-      <c r="N7">
+      <c r="P9">
         <v>0.7168486739469578</v>
       </c>
-      <c r="O7">
+      <c r="Q9">
         <v>0.2681451612903226</v>
       </c>
-      <c r="P7" t="s">
-        <v>36</v>
-      </c>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8">
-        <v>2.334321078864811</v>
-      </c>
-      <c r="F8">
-        <v>11445799.86329144</v>
-      </c>
-      <c r="G8">
-        <v>0.015</v>
-      </c>
-      <c r="H8">
-        <v>517</v>
-      </c>
-      <c r="I8">
-        <v>1042</v>
-      </c>
-      <c r="J8">
-        <v>13074</v>
-      </c>
-      <c r="K8">
-        <v>500</v>
-      </c>
-      <c r="L8">
-        <v>2.250963768001734</v>
-      </c>
-      <c r="M8">
-        <v>2.730328769708143</v>
-      </c>
-      <c r="N8">
-        <v>5.395018357323178</v>
-      </c>
-      <c r="O8">
-        <v>2.362586776421847</v>
-      </c>
-      <c r="P8" t="s">
-        <v>22</v>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10">
+        <v>0.6325136612021858</v>
+      </c>
+      <c r="F10">
+        <v>283425.2629285714</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10">
+        <v>463</v>
+      </c>
+      <c r="K10">
+        <v>381</v>
+      </c>
+      <c r="L10">
+        <v>1556</v>
+      </c>
+      <c r="M10">
+        <v>157</v>
+      </c>
+      <c r="N10">
+        <v>0.5485781990521327</v>
+      </c>
+      <c r="O10">
+        <v>0.7467741935483871</v>
+      </c>
+      <c r="P10">
+        <v>0.7895971842002346</v>
+      </c>
+      <c r="Q10">
+        <v>0.6325136612021858</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11">
+        <v>0.648854961832061</v>
+      </c>
+      <c r="F11">
+        <v>1248170.12208</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11">
+        <v>425</v>
+      </c>
+      <c r="K11">
+        <v>325</v>
+      </c>
+      <c r="L11">
+        <v>1679</v>
+      </c>
+      <c r="M11">
+        <v>135</v>
+      </c>
+      <c r="N11">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="O11">
+        <v>0.7589285714285714</v>
+      </c>
+      <c r="P11">
+        <v>0.8205928237129485</v>
+      </c>
+      <c r="Q11">
+        <v>0.648854961832061</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12">
+        <v>4.735248029346874</v>
+      </c>
+      <c r="F12">
+        <v>13285295.87294859</v>
+      </c>
+      <c r="G12">
+        <v>0.01075</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12">
+        <v>2029</v>
+      </c>
+      <c r="K12">
+        <v>2486</v>
+      </c>
+      <c r="L12">
+        <v>19833</v>
+      </c>
+      <c r="M12">
+        <v>1024</v>
+      </c>
+      <c r="N12">
+        <v>4.214615925451052</v>
+      </c>
+      <c r="O12">
+        <v>5.709383823515704</v>
+      </c>
+      <c r="P12">
+        <v>8.626164856191053</v>
+      </c>
+      <c r="Q12">
+        <v>4.735248029346874</v>
       </c>
     </row>
   </sheetData>

</xml_diff>